<commit_message>
Update ttest and boxplot - added function to divide feature into two and three subrange of depth - added ttest on subrange feature
</commit_message>
<xml_diff>
--- a/Results/2_T-test/ttest_summary.xlsx
+++ b/Results/2_T-test/ttest_summary.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNI\TESI\LAVORO TESI\Progetto_Matlab\Machine_Learning_Matlab_Studio_Abbondanza_Cetacei\Knowledge Discovery Process\Results\2_T-test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNI\TESI\LAVORO TESI\Progetto_Matlab\Machine Learning for Climate Change Application to Cetacean Abundance Studies\Results\2_T-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E85B569-D218-4837-AF4C-85461253045E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A676B4B5-FAA2-41D2-A1C4-373BE9B91E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10290" yWindow="5520" windowWidth="13380" windowHeight="15600" xr2:uid="{DA75F13D-7123-45B4-9FCC-BFDC1DCEB962}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{DA75F13D-7123-45B4-9FCC-BFDC1DCEB962}"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="All_Feature" sheetId="1" r:id="rId1"/>
+    <sheet name="Two_Subrange" sheetId="2" r:id="rId2"/>
+    <sheet name="Three_Subrange" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="151">
   <si>
     <t>Feature</t>
   </si>
@@ -415,6 +417,78 @@
   </si>
   <si>
     <t>3 su 16</t>
+  </si>
+  <si>
+    <t>temp_sup_50</t>
+  </si>
+  <si>
+    <t>temp_100_1000</t>
+  </si>
+  <si>
+    <t>prim_prod_sup_50</t>
+  </si>
+  <si>
+    <t>prim_prod_100_1000</t>
+  </si>
+  <si>
+    <t>nitrate_sup_50</t>
+  </si>
+  <si>
+    <t>nitrate_100_1000</t>
+  </si>
+  <si>
+    <t>phosphate_sup_50</t>
+  </si>
+  <si>
+    <t>phosphate_100_1000</t>
+  </si>
+  <si>
+    <t>salinity_sup_50</t>
+  </si>
+  <si>
+    <t>density_100_1000</t>
+  </si>
+  <si>
+    <t>density_sup_50</t>
+  </si>
+  <si>
+    <t>salinity_100_1000</t>
+  </si>
+  <si>
+    <t>temp_100_500</t>
+  </si>
+  <si>
+    <t>temp_600_1000</t>
+  </si>
+  <si>
+    <t>density_100_500</t>
+  </si>
+  <si>
+    <t>density_600_1000</t>
+  </si>
+  <si>
+    <t>salinity_100_500</t>
+  </si>
+  <si>
+    <t>salinity_600_1000</t>
+  </si>
+  <si>
+    <t>prim_prod_100_500</t>
+  </si>
+  <si>
+    <t>prim_prod_600_1000</t>
+  </si>
+  <si>
+    <t>nitrate_100_500</t>
+  </si>
+  <si>
+    <t>nitrate_600_1000</t>
+  </si>
+  <si>
+    <t>phosphate_100_500</t>
+  </si>
+  <si>
+    <t>phosphate_600_1000</t>
   </si>
 </sst>
 </file>
@@ -500,10 +574,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="17" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -826,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4700273-F075-4FA3-BA51-201C37FF9E66}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -899,13 +973,13 @@
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>117</v>
       </c>
     </row>
@@ -922,9 +996,9 @@
       <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -939,10 +1013,10 @@
       <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>115</v>
       </c>
       <c r="I5" s="6" t="s">
@@ -962,9 +1036,9 @@
       <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -979,9 +1053,9 @@
       <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -996,9 +1070,9 @@
       <c r="D8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1013,9 +1087,9 @@
       <c r="D9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1030,9 +1104,9 @@
       <c r="D10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1047,9 +1121,9 @@
       <c r="D11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1064,9 +1138,9 @@
       <c r="D12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1081,9 +1155,9 @@
       <c r="D13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1098,9 +1172,9 @@
       <c r="D14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1115,9 +1189,9 @@
       <c r="D15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1132,9 +1206,9 @@
       <c r="D16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -1149,9 +1223,9 @@
       <c r="D17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -1166,9 +1240,9 @@
       <c r="D18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -1183,9 +1257,9 @@
       <c r="D19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1200,9 +1274,9 @@
       <c r="D20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1217,13 +1291,13 @@
       <c r="D21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G21" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H21" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="4" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1240,9 +1314,9 @@
       <c r="D22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -1257,9 +1331,9 @@
       <c r="D23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1274,9 +1348,9 @@
       <c r="D24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -1291,9 +1365,9 @@
       <c r="D25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -1308,9 +1382,9 @@
       <c r="D26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -1325,9 +1399,9 @@
       <c r="D27" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -1342,9 +1416,9 @@
       <c r="D28" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
@@ -1359,9 +1433,9 @@
       <c r="D29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -1376,9 +1450,9 @@
       <c r="D30" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
@@ -1393,9 +1467,9 @@
       <c r="D31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
@@ -1410,9 +1484,9 @@
       <c r="D32" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
@@ -1427,9 +1501,9 @@
       <c r="D33" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
@@ -1444,9 +1518,9 @@
       <c r="D34" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
@@ -1461,9 +1535,9 @@
       <c r="D35" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
@@ -1478,9 +1552,9 @@
       <c r="D36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
@@ -1495,13 +1569,13 @@
       <c r="D37" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="G37" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="H37" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="I37" s="5" t="s">
+      <c r="I37" s="4" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1518,9 +1592,9 @@
       <c r="D38" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
@@ -1535,9 +1609,9 @@
       <c r="D39" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
@@ -1552,9 +1626,9 @@
       <c r="D40" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
@@ -1569,9 +1643,9 @@
       <c r="D41" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
@@ -1586,9 +1660,9 @@
       <c r="D42" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
@@ -1603,9 +1677,9 @@
       <c r="D43" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
@@ -1620,9 +1694,9 @@
       <c r="D44" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
@@ -1637,9 +1711,9 @@
       <c r="D45" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -1654,9 +1728,9 @@
       <c r="D46" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
@@ -1671,9 +1745,9 @@
       <c r="D47" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
@@ -1688,9 +1762,9 @@
       <c r="D48" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="5"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
@@ -1705,9 +1779,9 @@
       <c r="D49" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
@@ -1722,9 +1796,9 @@
       <c r="D50" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
@@ -1739,9 +1813,9 @@
       <c r="D51" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
@@ -1756,9 +1830,9 @@
       <c r="D52" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
@@ -1796,13 +1870,13 @@
       <c r="D54" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G54" s="5" t="s">
+      <c r="G54" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="H54" s="5" t="s">
+      <c r="H54" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="I54" s="5" t="s">
+      <c r="I54" s="4" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1819,9 +1893,9 @@
       <c r="D55" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
-      <c r="I55" s="5"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
@@ -1836,9 +1910,9 @@
       <c r="D56" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G56" s="5"/>
-      <c r="H56" s="5"/>
-      <c r="I56" s="5"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
@@ -1853,9 +1927,9 @@
       <c r="D57" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G57" s="5"/>
-      <c r="H57" s="5"/>
-      <c r="I57" s="5"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
@@ -1870,9 +1944,9 @@
       <c r="D58" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G58" s="5"/>
-      <c r="H58" s="5"/>
-      <c r="I58" s="5"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
@@ -1887,9 +1961,9 @@
       <c r="D59" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G59" s="5"/>
-      <c r="H59" s="5"/>
-      <c r="I59" s="5"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
@@ -1904,9 +1978,9 @@
       <c r="D60" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
@@ -1921,9 +1995,9 @@
       <c r="D61" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
-      <c r="I61" s="5"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
@@ -1938,9 +2012,9 @@
       <c r="D62" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G62" s="5"/>
-      <c r="H62" s="5"/>
-      <c r="I62" s="5"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
@@ -1955,9 +2029,9 @@
       <c r="D63" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
@@ -1972,9 +2046,9 @@
       <c r="D64" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G64" s="5"/>
-      <c r="H64" s="5"/>
-      <c r="I64" s="5"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
@@ -1989,9 +2063,9 @@
       <c r="D65" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
-      <c r="I65" s="5"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
@@ -2006,9 +2080,9 @@
       <c r="D66" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G66" s="5"/>
-      <c r="H66" s="5"/>
-      <c r="I66" s="5"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
@@ -2023,9 +2097,9 @@
       <c r="D67" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G67" s="5"/>
-      <c r="H67" s="5"/>
-      <c r="I67" s="5"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
@@ -2040,9 +2114,9 @@
       <c r="D68" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G68" s="5"/>
-      <c r="H68" s="5"/>
-      <c r="I68" s="5"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
@@ -2057,9 +2131,9 @@
       <c r="D69" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
-      <c r="I69" s="5"/>
+      <c r="G69" s="4"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="4"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
@@ -2074,13 +2148,13 @@
       <c r="D70" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G70" s="5" t="s">
+      <c r="G70" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="H70" s="5" t="s">
+      <c r="H70" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="I70" s="5" t="s">
+      <c r="I70" s="4" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2097,9 +2171,9 @@
       <c r="D71" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G71" s="5"/>
-      <c r="H71" s="5"/>
-      <c r="I71" s="5"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
@@ -2114,9 +2188,9 @@
       <c r="D72" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G72" s="5"/>
-      <c r="H72" s="5"/>
-      <c r="I72" s="5"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
@@ -2131,9 +2205,9 @@
       <c r="D73" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
-      <c r="I73" s="5"/>
+      <c r="G73" s="4"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
@@ -2148,9 +2222,9 @@
       <c r="D74" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
-      <c r="I74" s="5"/>
+      <c r="G74" s="4"/>
+      <c r="H74" s="4"/>
+      <c r="I74" s="4"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
@@ -2165,9 +2239,9 @@
       <c r="D75" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G75" s="5"/>
-      <c r="H75" s="5"/>
-      <c r="I75" s="5"/>
+      <c r="G75" s="4"/>
+      <c r="H75" s="4"/>
+      <c r="I75" s="4"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
@@ -2182,9 +2256,9 @@
       <c r="D76" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G76" s="5"/>
-      <c r="H76" s="5"/>
-      <c r="I76" s="5"/>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
@@ -2199,9 +2273,9 @@
       <c r="D77" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G77" s="5"/>
-      <c r="H77" s="5"/>
-      <c r="I77" s="5"/>
+      <c r="G77" s="4"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="4"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
@@ -2216,9 +2290,9 @@
       <c r="D78" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G78" s="5"/>
-      <c r="H78" s="5"/>
-      <c r="I78" s="5"/>
+      <c r="G78" s="4"/>
+      <c r="H78" s="4"/>
+      <c r="I78" s="4"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
@@ -2233,9 +2307,9 @@
       <c r="D79" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G79" s="5"/>
-      <c r="H79" s="5"/>
-      <c r="I79" s="5"/>
+      <c r="G79" s="4"/>
+      <c r="H79" s="4"/>
+      <c r="I79" s="4"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
@@ -2250,9 +2324,9 @@
       <c r="D80" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G80" s="5"/>
-      <c r="H80" s="5"/>
-      <c r="I80" s="5"/>
+      <c r="G80" s="4"/>
+      <c r="H80" s="4"/>
+      <c r="I80" s="4"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
@@ -2267,9 +2341,9 @@
       <c r="D81" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G81" s="5"/>
-      <c r="H81" s="5"/>
-      <c r="I81" s="5"/>
+      <c r="G81" s="4"/>
+      <c r="H81" s="4"/>
+      <c r="I81" s="4"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
@@ -2284,9 +2358,9 @@
       <c r="D82" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G82" s="5"/>
-      <c r="H82" s="5"/>
-      <c r="I82" s="5"/>
+      <c r="G82" s="4"/>
+      <c r="H82" s="4"/>
+      <c r="I82" s="4"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
@@ -2301,9 +2375,9 @@
       <c r="D83" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G83" s="5"/>
-      <c r="H83" s="5"/>
-      <c r="I83" s="5"/>
+      <c r="G83" s="4"/>
+      <c r="H83" s="4"/>
+      <c r="I83" s="4"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
@@ -2318,9 +2392,9 @@
       <c r="D84" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G84" s="5"/>
-      <c r="H84" s="5"/>
-      <c r="I84" s="5"/>
+      <c r="G84" s="4"/>
+      <c r="H84" s="4"/>
+      <c r="I84" s="4"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
@@ -2335,9 +2409,9 @@
       <c r="D85" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G85" s="5"/>
-      <c r="H85" s="5"/>
-      <c r="I85" s="5"/>
+      <c r="G85" s="4"/>
+      <c r="H85" s="4"/>
+      <c r="I85" s="4"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
@@ -2352,13 +2426,13 @@
       <c r="D86" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G86" s="5" t="s">
+      <c r="G86" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="H86" s="5" t="s">
+      <c r="H86" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="I86" s="5" t="s">
+      <c r="I86" s="4" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2375,9 +2449,9 @@
       <c r="D87" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G87" s="5"/>
-      <c r="H87" s="5"/>
-      <c r="I87" s="5"/>
+      <c r="G87" s="4"/>
+      <c r="H87" s="4"/>
+      <c r="I87" s="4"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
@@ -2392,9 +2466,9 @@
       <c r="D88" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G88" s="5"/>
-      <c r="H88" s="5"/>
-      <c r="I88" s="5"/>
+      <c r="G88" s="4"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="4"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
@@ -2409,9 +2483,9 @@
       <c r="D89" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G89" s="5"/>
-      <c r="H89" s="5"/>
-      <c r="I89" s="5"/>
+      <c r="G89" s="4"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="4"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
@@ -2426,9 +2500,9 @@
       <c r="D90" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G90" s="5"/>
-      <c r="H90" s="5"/>
-      <c r="I90" s="5"/>
+      <c r="G90" s="4"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="4"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
@@ -2443,9 +2517,9 @@
       <c r="D91" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G91" s="5"/>
-      <c r="H91" s="5"/>
-      <c r="I91" s="5"/>
+      <c r="G91" s="4"/>
+      <c r="H91" s="4"/>
+      <c r="I91" s="4"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
@@ -2460,9 +2534,9 @@
       <c r="D92" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G92" s="5"/>
-      <c r="H92" s="5"/>
-      <c r="I92" s="5"/>
+      <c r="G92" s="4"/>
+      <c r="H92" s="4"/>
+      <c r="I92" s="4"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
@@ -2477,9 +2551,9 @@
       <c r="D93" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G93" s="5"/>
-      <c r="H93" s="5"/>
-      <c r="I93" s="5"/>
+      <c r="G93" s="4"/>
+      <c r="H93" s="4"/>
+      <c r="I93" s="4"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
@@ -2494,9 +2568,9 @@
       <c r="D94" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G94" s="5"/>
-      <c r="H94" s="5"/>
-      <c r="I94" s="5"/>
+      <c r="G94" s="4"/>
+      <c r="H94" s="4"/>
+      <c r="I94" s="4"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
@@ -2511,9 +2585,9 @@
       <c r="D95" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G95" s="5"/>
-      <c r="H95" s="5"/>
-      <c r="I95" s="5"/>
+      <c r="G95" s="4"/>
+      <c r="H95" s="4"/>
+      <c r="I95" s="4"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
@@ -2528,9 +2602,9 @@
       <c r="D96" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G96" s="5"/>
-      <c r="H96" s="5"/>
-      <c r="I96" s="5"/>
+      <c r="G96" s="4"/>
+      <c r="H96" s="4"/>
+      <c r="I96" s="4"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
@@ -2545,9 +2619,9 @@
       <c r="D97" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G97" s="5"/>
-      <c r="H97" s="5"/>
-      <c r="I97" s="5"/>
+      <c r="G97" s="4"/>
+      <c r="H97" s="4"/>
+      <c r="I97" s="4"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
@@ -2562,9 +2636,9 @@
       <c r="D98" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G98" s="5"/>
-      <c r="H98" s="5"/>
-      <c r="I98" s="5"/>
+      <c r="G98" s="4"/>
+      <c r="H98" s="4"/>
+      <c r="I98" s="4"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
@@ -2579,9 +2653,9 @@
       <c r="D99" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G99" s="5"/>
-      <c r="H99" s="5"/>
-      <c r="I99" s="5"/>
+      <c r="G99" s="4"/>
+      <c r="H99" s="4"/>
+      <c r="I99" s="4"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
@@ -2596,9 +2670,9 @@
       <c r="D100" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G100" s="5"/>
-      <c r="H100" s="5"/>
-      <c r="I100" s="5"/>
+      <c r="G100" s="4"/>
+      <c r="H100" s="4"/>
+      <c r="I100" s="4"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
@@ -2613,24 +2687,12 @@
       <c r="D101" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G101" s="5"/>
-      <c r="H101" s="5"/>
-      <c r="I101" s="5"/>
+      <c r="G101" s="4"/>
+      <c r="H101" s="4"/>
+      <c r="I101" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G70:G85"/>
-    <mergeCell ref="H70:H85"/>
-    <mergeCell ref="I70:I85"/>
-    <mergeCell ref="G86:G101"/>
-    <mergeCell ref="H86:H101"/>
-    <mergeCell ref="I86:I101"/>
-    <mergeCell ref="G37:G52"/>
-    <mergeCell ref="H37:H52"/>
-    <mergeCell ref="I37:I52"/>
-    <mergeCell ref="G54:G69"/>
-    <mergeCell ref="H54:H69"/>
-    <mergeCell ref="I54:I69"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="G5:G20"/>
     <mergeCell ref="H5:H20"/>
@@ -2640,9 +2702,510 @@
     <mergeCell ref="I21:I36"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="I3:I4"/>
+    <mergeCell ref="G37:G52"/>
+    <mergeCell ref="H37:H52"/>
+    <mergeCell ref="I37:I52"/>
+    <mergeCell ref="G54:G69"/>
+    <mergeCell ref="H54:H69"/>
+    <mergeCell ref="I54:I69"/>
+    <mergeCell ref="G70:G85"/>
+    <mergeCell ref="H70:H85"/>
+    <mergeCell ref="I70:I85"/>
+    <mergeCell ref="G86:G101"/>
+    <mergeCell ref="H86:H101"/>
+    <mergeCell ref="I86:I101"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21DACF8D-85BB-435E-8644-E3E854CD42D4}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF9B2CD-E2D1-40D7-AB50-6508FB035DCB}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="4" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>